<commit_message>
Add RoomDataLoader and RoomType classes with CSV loading functionality
</commit_message>
<xml_diff>
--- a/liste salles.xlsx
+++ b/liste salles.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\Cours 3A\Market design\classroom_allocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D1A76A-8DB7-4688-8F8E-9069F02CF474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EC037A-C22F-431E-A923-11ADA79D858C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{530261B0-E9DD-4B7F-97AD-3C43C5023888}"/>
+    <workbookView xWindow="30330" yWindow="390" windowWidth="25185" windowHeight="14265" xr2:uid="{530261B0-E9DD-4B7F-97AD-3C43C5023888}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="89">
   <si>
     <t>Room/Amphi</t>
   </si>
@@ -194,9 +194,6 @@
     <t>salle info 36</t>
   </si>
   <si>
-    <t>Türing</t>
-  </si>
-  <si>
     <t>Salle langues 51</t>
   </si>
   <si>
@@ -276,13 +273,46 @@
   </si>
   <si>
     <t>Monge</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Salles info</t>
+  </si>
+  <si>
+    <t>Salles langues</t>
+  </si>
+  <si>
+    <t>Nouveaux amphis</t>
+  </si>
+  <si>
+    <t>Grands amphis</t>
+  </si>
+  <si>
+    <t>couloir de la scolarité</t>
+  </si>
+  <si>
+    <t>Amphi couloir binets</t>
+  </si>
+  <si>
+    <t>couloir des labos</t>
+  </si>
+  <si>
+    <t>Salles 100</t>
+  </si>
+  <si>
+    <t>Amphis 80-100 places</t>
+  </si>
+  <si>
+    <t>Couloir cour Vanneau</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +324,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -656,643 +692,868 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E418269A-FE49-4620-A4E4-8AB0F7C3E295}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33">
         <v>42</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37">
         <v>28</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38">
         <v>28</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39">
         <v>31</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40">
         <v>48</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
         <v>48</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44">
         <v>18</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47">
         <v>24</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48">
         <v>24</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49">
         <v>24</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50">
         <v>24</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52">
         <v>18</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="C53" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57">
         <v>18</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="C58" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="C59" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C60" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C61" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="C62" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+      <c r="C63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64">
         <v>50</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C64" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65">
         <v>50</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66">
         <v>50</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C66" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67">
         <v>50</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68">
         <v>50</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C68" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+        <v>780</v>
+      </c>
+      <c r="C69" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+        <v>523</v>
+      </c>
+      <c r="C70" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+      <c r="C71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+        <v>230</v>
+      </c>
+      <c r="C72" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+      <c r="C73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="C74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="C75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="C76" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77">
         <v>81</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>78</v>
-      </c>
-      <c r="B78">
-        <v>81</v>
+      <c r="C77" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B69" xr:uid="{E418269A-FE49-4620-A4E4-8AB0F7C3E295}"/>
+  <autoFilter ref="A1:B68" xr:uid="{E418269A-FE49-4620-A4E4-8AB0F7C3E295}"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>